<commit_message>
Add parts.csv for testing
</commit_message>
<xml_diff>
--- a/templates/Work Pak Part_template.xlsx
+++ b/templates/Work Pak Part_template.xlsx
@@ -1,19 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Implementation\_CORRIDOR IMPLEMENTATION FILES\CorImport\v11.8\Work Pak data templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csundbeck\Documents\Dev\CorImport Web Tool\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{250596CA-8BEC-419E-8D0E-9F35622CA4DA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6825" yWindow="2055" windowWidth="21600" windowHeight="11835"/>
   </bookViews>
   <sheets>
-    <sheet name="11.5 Add Update Work Pak_Part_d" sheetId="1" r:id="rId1"/>
+    <sheet name="Work Pak Part_template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -58,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>

</xml_diff>